<commit_message>
get_queue_items workflow made, Get_Hotels uses info from queue to get results
</commit_message>
<xml_diff>
--- a/customerqueue/rdtr1.xlsx
+++ b/customerqueue/rdtr1.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\customerqueue\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0B5AA5-2427-4338-8843-862A3EAA2DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="24" windowWidth="16260" windowHeight="6384"/>
+    <workbookView xWindow="5220" yWindow="2340" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rdt1.xlsx" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -46,16 +52,37 @@
     <t>Rich Drexel</t>
   </si>
   <si>
-    <t>Dallas, TX</t>
-  </si>
-  <si>
-    <t>London, UK</t>
+    <t>Dallas, Texas, United States of America</t>
+  </si>
+  <si>
+    <t>Paris, France</t>
+  </si>
+  <si>
+    <t>$100 to $299</t>
+  </si>
+  <si>
+    <t>More than $500</t>
+  </si>
+  <si>
+    <t>2 Rooms</t>
+  </si>
+  <si>
+    <t>1 Room</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="mm/dd/yyyy;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -536,7 +563,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -588,6 +615,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -635,7 +665,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -668,9 +698,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -703,6 +750,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -878,14 +942,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -923,8 +990,8 @@
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
-        <v>10000</v>
+      <c r="C2" t="s">
+        <v>12</v>
       </c>
       <c r="D2" s="1">
         <v>45037</v>
@@ -935,14 +1002,14 @@
       <c r="F2">
         <v>4</v>
       </c>
-      <c r="G2">
-        <v>2</v>
+      <c r="G2" t="s">
+        <v>14</v>
       </c>
       <c r="H2">
         <v>3</v>
       </c>
-      <c r="I2" t="b">
-        <v>0</v>
+      <c r="I2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -952,8 +1019,8 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3">
-        <v>15000</v>
+      <c r="C3" t="s">
+        <v>13</v>
       </c>
       <c r="D3" s="1">
         <v>45237</v>
@@ -964,17 +1031,18 @@
       <c r="F3">
         <v>4</v>
       </c>
-      <c r="G3">
-        <v>2</v>
+      <c r="G3" t="s">
+        <v>15</v>
       </c>
       <c r="H3">
         <v>4</v>
       </c>
-      <c r="I3" t="b">
-        <v>0</v>
+      <c r="I3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>